<commit_message>
novos resultados e resultado falho
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -77,12 +77,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="17">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -101,21 +100,139 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -123,8 +240,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,6 +280,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -158,23 +341,100 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -186,7 +446,7 @@
   <dimension ref="D6:H36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -389,17 +649,27 @@
       <c r="E25" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H25" s="1" t="n">
+        <v>613325</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="3"/>
       <c r="E26" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H26" s="1" t="n">
+        <v>298611</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="3"/>
       <c r="E27" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <f aca="false">921557 - SUM(H25:H26)</f>
+        <v>9621</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fotos de valor e resultados reais
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -77,11 +77,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -100,139 +101,21 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -240,23 +123,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,57 +148,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -341,100 +158,23 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -446,7 +186,7 @@
   <dimension ref="D6:H36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -629,17 +369,27 @@
       <c r="E22" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H22" s="1" t="n">
+        <v>321820</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="3"/>
       <c r="E23" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H23" s="1" t="n">
+        <v>525551</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="3"/>
       <c r="E24" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <f aca="false">921571 - SUM(H22:H23)</f>
+        <v>74200</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
resultados e legendas novas
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -200,10 +200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D6:M46"/>
+  <dimension ref="D6:R46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -212,10 +212,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.34"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,6 +280,9 @@
         <v>7</v>
       </c>
       <c r="G10" s="0"/>
+      <c r="H10" s="0" t="n">
+        <v>6.19</v>
+      </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,6 +304,13 @@
       <c r="M11" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="Q11" s="0" t="n">
+        <f aca="false">SUM(H32:H33)</f>
+        <v>33.45</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="3"/>
@@ -318,6 +330,13 @@
         <f aca="false">(M11*L12)/L11</f>
         <v>32.4028790405802</v>
       </c>
+      <c r="Q12" s="0" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="R12" s="5" t="n">
+        <f aca="false">(R11*Q12)/Q11</f>
+        <v>3.1390134529148</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="3"/>
@@ -338,6 +357,9 @@
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H14" s="0" t="n">
+        <v>9.06</v>
+      </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -385,6 +407,9 @@
       <c r="E18" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H18" s="0" t="n">
+        <v>6.33</v>
+      </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,6 +457,9 @@
       <c r="E22" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H22" s="0" t="n">
+        <v>11.89</v>
+      </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,6 +507,9 @@
       <c r="E26" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H26" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,6 +557,9 @@
       <c r="E30" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H30" s="0" t="n">
+        <v>12.37</v>
+      </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,6 +606,9 @@
       <c r="D34" s="3"/>
       <c r="E34" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>3.14</v>
       </c>
       <c r="I34" s="1"/>
     </row>

</xml_diff>

<commit_message>
todos os resultados até agoraforma computados
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="27">
   <si>
     <t xml:space="preserve">RGB</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">GIMP</t>
   </si>
   <si>
+    <t xml:space="preserve">Severidade da Doença</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foto 1</t>
   </si>
   <si>
@@ -43,9 +46,6 @@
     <t xml:space="preserve">Doença</t>
   </si>
   <si>
-    <t xml:space="preserve">Severidade da Doença</t>
-  </si>
-  <si>
     <t xml:space="preserve">Foto 2</t>
   </si>
   <si>
@@ -71,6 +71,36 @@
   </si>
   <si>
     <t xml:space="preserve">Foto 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto 20</t>
   </si>
 </sst>
 </file>
@@ -154,7 +184,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -169,6 +199,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -204,10 +238,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D6:T46"/>
+  <dimension ref="D6:T66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K44" activeCellId="0" sqref="K44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O26" activeCellId="0" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -215,10 +249,11 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="7.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.07"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="7.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="14" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11.52"/>
@@ -234,13 +269,18 @@
       <c r="H6" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="K6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">100-SUM(F8:F9)</f>
@@ -253,6 +293,15 @@
       <c r="H7" s="0" t="n">
         <v>82.23</v>
       </c>
+      <c r="K7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="T7" s="1" t="n">
         <v>757273</v>
       </c>
@@ -260,7 +309,7 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="3"/>
       <c r="E8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>13.28</v>
@@ -270,6 +319,18 @@
       </c>
       <c r="H8" s="0" t="n">
         <v>16.67</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>0.1762</v>
+      </c>
+      <c r="L8" s="6" t="n">
+        <v>0.2043</v>
+      </c>
+      <c r="M8" s="6" t="n">
+        <v>0.0619</v>
       </c>
       <c r="T8" s="1" t="n">
         <v>153490</v>
@@ -278,7 +339,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="3"/>
       <c r="E9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.84</v>
@@ -290,47 +351,83 @@
         <f aca="false">100-SUM(H7:H8)</f>
         <v>1.09999999999999</v>
       </c>
+      <c r="J9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>0.2309</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>0.2669</v>
+      </c>
+      <c r="M9" s="6" t="n">
+        <v>0.0906</v>
+      </c>
       <c r="T9" s="1" t="n">
         <f aca="false">920910 - SUM(T7:T8)</f>
         <v>10147</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="4" t="n">
-        <v>0.1762</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>0.2043</v>
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <f aca="false">100-SUM(F11:F12)</f>
+        <v>57.51</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <f aca="false">100-SUM(G11:G12)</f>
+        <v>57.52</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>6.19</v>
+        <v>57.62</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>0.3213</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <v>0.422</v>
+      </c>
+      <c r="M10" s="6" t="n">
+        <v>0.0633</v>
       </c>
       <c r="T10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="D11" s="3"/>
       <c r="E11" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F11" s="1" t="n">
-        <f aca="false">100-SUM(F12:F13)</f>
-        <v>57.51</v>
+        <v>32.68</v>
       </c>
       <c r="G11" s="1" t="n">
-        <f aca="false">100-SUM(G12:G13)</f>
-        <v>57.52</v>
+        <v>31.14</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>57.62</v>
+        <v>38.54</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>0.3166</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <v>0.3656</v>
+      </c>
+      <c r="M11" s="6" t="n">
+        <v>0.1189</v>
       </c>
       <c r="Q11" s="0" t="n">
-        <f aca="false">SUM(H32:H33)</f>
+        <f aca="false">SUM(H26:H27)</f>
         <v>33.45</v>
       </c>
       <c r="R11" s="0" t="n">
@@ -343,21 +440,34 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="3"/>
       <c r="E12" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>32.68</v>
+        <v>9.81</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>31.14</v>
+        <v>11.34</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>38.54</v>
+        <f aca="false">100-SUM(H10:H11)</f>
+        <v>3.84</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>0.3058</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <v>0.3528</v>
+      </c>
+      <c r="M12" s="6" t="n">
+        <v>0.03</v>
       </c>
       <c r="Q12" s="0" t="n">
         <v>1.05</v>
       </c>
-      <c r="R12" s="6" t="n">
+      <c r="R12" s="7" t="n">
         <f aca="false">(R11*Q12)/Q11</f>
         <v>3.1390134529148</v>
       </c>
@@ -366,19 +476,34 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>9.81</v>
+        <f aca="false">100-SUM(F14:F15)</f>
+        <v>79.55</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>11.34</v>
+        <f aca="false">100-SUM(G14:G15)</f>
+        <v>79.55</v>
       </c>
       <c r="H13" s="0" t="n">
-        <f aca="false">100-SUM(H11:H12)</f>
-        <v>3.84</v>
+        <v>79.63</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <v>0.3159</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <v>0.3668</v>
+      </c>
+      <c r="M13" s="6" t="n">
+        <v>0.1237</v>
       </c>
       <c r="T13" s="1" t="n">
         <f aca="false">921359 - SUM(T11:T12)</f>
@@ -388,18 +513,30 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="3"/>
       <c r="E14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="4" t="n">
-        <v>0.2309</v>
-      </c>
-      <c r="G14" s="4" t="n">
-        <v>0.2669</v>
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>13.88</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>11.82</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>9.06</v>
-      </c>
-      <c r="Q14" s="7" t="n">
+        <v>19.08</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <v>0.5323</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="M14" s="6" t="n">
+        <v>0.0314</v>
+      </c>
+      <c r="Q14" s="8" t="n">
         <v>921557</v>
       </c>
       <c r="R14" s="0" t="n">
@@ -408,27 +545,27 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F15" s="1" t="n">
-        <f aca="false">100-SUM(F16:F17)</f>
-        <v>100</v>
+        <v>6.57</v>
       </c>
       <c r="G15" s="1" t="n">
-        <f aca="false">100-SUM(G16:G17)</f>
-        <v>100</v>
+        <v>8.63</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>79.63</v>
+        <f aca="false">100-SUM(H13:H14)</f>
+        <v>1.29000000000001</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="Q15" s="1" t="n">
         <v>298611</v>
       </c>
-      <c r="R15" s="6" t="n">
+      <c r="R15" s="7" t="n">
         <f aca="false">(R14*Q15)/Q14</f>
         <v>32.4028790405802</v>
       </c>
@@ -437,12 +574,25 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F16" s="1" t="n">
+        <f aca="false">100-SUM(F17:F18)</f>
+        <v>35.06</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">100-SUM(G17:G18)</f>
+        <v>35.07</v>
+      </c>
       <c r="H16" s="0" t="n">
-        <v>19.08</v>
+        <v>35.07</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="T16" s="1" t="n">
         <v>175831</v>
@@ -453,9 +603,17 @@
       <c r="E17" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F17" s="1" t="n">
+        <v>44.38</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>41.19</v>
+      </c>
       <c r="H17" s="0" t="n">
-        <f aca="false">100-SUM(H15:H16)</f>
-        <v>1.29000000000001</v>
+        <v>57.21</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="T17" s="1" t="n">
         <f aca="false">921600 - SUM(T15:T16)</f>
@@ -467,28 +625,41 @@
       <c r="E18" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F18" s="1" t="n">
+        <v>20.56</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>23.74</v>
+      </c>
       <c r="H18" s="0" t="n">
-        <v>6.33</v>
+        <f aca="false">100-SUM(H16:H17)</f>
+        <v>7.72</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="T18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">100-SUM(F20:F21)</f>
-        <v>100</v>
+        <v>65.7</v>
       </c>
       <c r="G19" s="1" t="n">
         <f aca="false">100-SUM(G20:G21)</f>
-        <v>100</v>
+        <v>65.7</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>35.07</v>
+        <v>65.7</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="T19" s="1" t="n">
         <v>323160</v>
@@ -497,10 +668,19 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="3"/>
       <c r="E20" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>23.81</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>22.2</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>57.21</v>
+        <v>33.27</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="T20" s="1" t="n">
         <v>527281</v>
@@ -509,11 +689,20 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="3"/>
       <c r="E21" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>12.1</v>
       </c>
       <c r="H21" s="0" t="n">
         <f aca="false">100-SUM(H19:H20)</f>
-        <v>7.72</v>
+        <v>1.03</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="T21" s="1" t="n">
         <f aca="false">921582 - SUM(T19:T20)</f>
@@ -521,32 +710,44 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E22" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <f aca="false">100-SUM(F23:F24)</f>
+        <v>34.92</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <f aca="false">100-SUM(G23:G24)</f>
+        <v>34.92</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>11.89</v>
+        <v>34.92</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="T22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F23" s="1" t="n">
-        <f aca="false">100-SUM(F24:F25)</f>
-        <v>100</v>
+        <v>44.52</v>
       </c>
       <c r="G23" s="1" t="n">
-        <f aca="false">100-SUM(G24:G25)</f>
-        <v>100</v>
+        <v>41.21</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>65.7</v>
+        <v>57.03</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="T23" s="1" t="n">
         <v>605471</v>
@@ -555,23 +756,45 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="3"/>
       <c r="E24" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>20.56</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>23.87</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>33.27</v>
+        <f aca="false">100-SUM(H22:H23)</f>
+        <v>8.05</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="T24" s="1" t="n">
         <v>306577</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="E25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <f aca="false">100-SUM(F26:F27)</f>
+        <v>66.56</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <f aca="false">100-SUM(G26:G27)</f>
+        <v>66.56</v>
       </c>
       <c r="H25" s="0" t="n">
-        <f aca="false">100-SUM(H23:H24)</f>
-        <v>1.03</v>
+        <v>66.55</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="T25" s="1" t="n">
         <f aca="false">921578 - SUM(T23:T24)</f>
@@ -581,42 +804,58 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="3"/>
       <c r="E26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>15.64</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>11.87</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>3</v>
+        <v>32.4</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="T26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F27" s="1" t="n">
-        <f aca="false">100-SUM(F28:F29)</f>
-        <v>100</v>
+        <v>17.8</v>
       </c>
       <c r="G27" s="1" t="n">
-        <f aca="false">100-SUM(G28:G29)</f>
-        <v>100</v>
+        <v>21.57</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>34.92</v>
+        <f aca="false">100-SUM(H25:H26)</f>
+        <v>1.05000000000001</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="T27" s="1" t="n">
         <v>321820</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="0" t="n">
-        <v>57.03</v>
+      <c r="F28" s="1" t="n">
+        <f aca="false">100-SUM(F29:F30)</f>
+        <v>100</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <f aca="false">100-SUM(G29:G30)</f>
+        <v>100</v>
       </c>
       <c r="T28" s="1" t="n">
         <v>525551</v>
@@ -627,10 +866,6 @@
       <c r="E29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="0" t="n">
-        <f aca="false">100-SUM(H27:H28)</f>
-        <v>8.05</v>
-      </c>
       <c r="T29" s="1" t="n">
         <f aca="false">921571 - SUM(T27:T28)</f>
         <v>74200</v>
@@ -642,16 +877,17 @@
         <v>7</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>12.37</v>
+        <f aca="false">100-SUM(H28:H29)</f>
+        <v>100</v>
       </c>
       <c r="T30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F31" s="1" t="n">
         <f aca="false">100-SUM(F32:F33)</f>
@@ -660,9 +896,6 @@
       <c r="G31" s="1" t="n">
         <f aca="false">100-SUM(G32:G33)</f>
         <v>100</v>
-      </c>
-      <c r="H31" s="0" t="n">
-        <v>66.55</v>
       </c>
       <c r="T31" s="1" t="n">
         <v>613325</v>
@@ -671,10 +904,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="3"/>
       <c r="E32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="0" t="n">
-        <v>32.4</v>
+        <v>6</v>
       </c>
       <c r="T32" s="1" t="n">
         <v>298611</v>
@@ -683,11 +913,11 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="3"/>
       <c r="E33" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H33" s="0" t="n">
         <f aca="false">100-SUM(H31:H32)</f>
-        <v>1.05000000000001</v>
+        <v>100</v>
       </c>
       <c r="T33" s="1" t="n">
         <f aca="false">921557 - SUM(T31:T32)</f>
@@ -695,46 +925,53 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="E34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="0" t="n">
-        <v>3.14</v>
+        <v>5</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <f aca="false">100-SUM(F35:F36)</f>
+        <v>100</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <f aca="false">100-SUM(G35:G36)</f>
+        <v>100</v>
       </c>
       <c r="I34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="D35" s="3"/>
       <c r="E35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="1" t="n">
-        <f aca="false">100-SUM(F36:F37)</f>
-        <v>100</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <f aca="false">100-SUM(G36:G37)</f>
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="I35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D36" s="3"/>
       <c r="E36" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <f aca="false">100-SUM(H34:H35)</f>
+        <v>100</v>
       </c>
       <c r="I36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="E37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" s="0" t="n">
-        <f aca="false">100-SUM(H35:H36)</f>
+        <v>5</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <f aca="false">100-SUM(F38:F39)</f>
+        <v>100</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <f aca="false">100-SUM(G38:G39)</f>
         <v>100</v>
       </c>
       <c r="I37" s="1"/>
@@ -742,31 +979,35 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="3"/>
       <c r="E38" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="D39" s="3"/>
       <c r="E39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="1" t="n">
-        <f aca="false">100-SUM(F40:F41)</f>
-        <v>100</v>
-      </c>
-      <c r="G39" s="1" t="n">
-        <f aca="false">100-SUM(G40:G41)</f>
+        <v>7</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <f aca="false">100-SUM(H37:H38)</f>
         <v>100</v>
       </c>
       <c r="I39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <f aca="false">100-SUM(F41:F42)</f>
+        <v>100</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <f aca="false">100-SUM(G41:G42)</f>
+        <v>100</v>
       </c>
       <c r="I40" s="1"/>
     </row>
@@ -775,10 +1016,6 @@
       <c r="E41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H41" s="0" t="n">
-        <f aca="false">100-SUM(H39:H40)</f>
-        <v>100</v>
-      </c>
       <c r="I41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,14 +1023,18 @@
       <c r="E42" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H42" s="0" t="n">
+        <f aca="false">100-SUM(H40:H41)</f>
+        <v>100</v>
+      </c>
       <c r="I42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F43" s="1" t="n">
         <f aca="false">100-SUM(F44:F45)</f>
@@ -808,14 +1049,14 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="3"/>
       <c r="E44" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="3"/>
       <c r="E45" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H45" s="0" t="n">
         <f aca="false">100-SUM(H43:H44)</f>
@@ -824,24 +1065,253 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="E46" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <f aca="false">100-SUM(F47:F48)</f>
+        <v>100</v>
+      </c>
+      <c r="G46" s="1" t="n">
+        <f aca="false">100-SUM(G47:G48)</f>
+        <v>100</v>
       </c>
       <c r="I46" s="1"/>
     </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D47" s="3"/>
+      <c r="E47" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D48" s="3"/>
+      <c r="E48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <f aca="false">100-SUM(H46:H47)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D49" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <f aca="false">100-SUM(F50:F51)</f>
+        <v>100</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <f aca="false">100-SUM(G50:G51)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D50" s="3"/>
+      <c r="E50" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D51" s="3"/>
+      <c r="E51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <f aca="false">100-SUM(H49:H50)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <f aca="false">100-SUM(F53:F54)</f>
+        <v>100</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <f aca="false">100-SUM(G53:G54)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D53" s="3"/>
+      <c r="E53" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D54" s="3"/>
+      <c r="E54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <f aca="false">100-SUM(H52:H53)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D55" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <f aca="false">100-SUM(F56:F57)</f>
+        <v>100</v>
+      </c>
+      <c r="G55" s="1" t="n">
+        <f aca="false">100-SUM(G56:G57)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D56" s="3"/>
+      <c r="E56" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D57" s="3"/>
+      <c r="E57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <f aca="false">100-SUM(H55:H56)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D58" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <f aca="false">100-SUM(F59:F60)</f>
+        <v>100</v>
+      </c>
+      <c r="G58" s="1" t="n">
+        <f aca="false">100-SUM(G59:G60)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D59" s="3"/>
+      <c r="E59" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D60" s="3"/>
+      <c r="E60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <f aca="false">100-SUM(H58:H59)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="1" t="n">
+        <f aca="false">100-SUM(F62:F63)</f>
+        <v>100</v>
+      </c>
+      <c r="G61" s="1" t="n">
+        <f aca="false">100-SUM(G62:G63)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D62" s="3"/>
+      <c r="E62" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="3"/>
+      <c r="E63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <f aca="false">100-SUM(H61:H62)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D64" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" s="1" t="n">
+        <f aca="false">100-SUM(F65:F66)</f>
+        <v>100</v>
+      </c>
+      <c r="G64" s="1" t="n">
+        <f aca="false">100-SUM(G65:G66)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D65" s="3"/>
+      <c r="E65" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D66" s="3"/>
+      <c r="E66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <f aca="false">100-SUM(H64:H65)</f>
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="D43:D46"/>
+  <mergeCells count="21">
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="D64:D66"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Novas fotos e resultados
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="42">
   <si>
     <t xml:space="preserve">RGB</t>
   </si>
@@ -296,8 +296,8 @@
   </sheetPr>
   <dimension ref="D6:T36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N25" activeCellId="0" sqref="N25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N20" activeCellId="1" sqref="M5:R5 N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -309,10 +309,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="7.68"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="19" style="0" width="11.52"/>
@@ -1051,10 +1050,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D4:I29"/>
+  <dimension ref="C4:R29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1083,6 +1082,24 @@
       <c r="I4" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="M4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="4" t="s">
@@ -1103,8 +1120,32 @@
       <c r="I5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="L5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="n">
+        <v>16</v>
+      </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1122,6 +1163,24 @@
       </c>
       <c r="I6" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,6 +1202,24 @@
       <c r="I7" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="M7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="4" t="s">
@@ -1163,6 +1240,24 @@
       <c r="I8" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="M8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="4" t="s">
@@ -1183,6 +1278,24 @@
       <c r="I9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="M9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="4" t="s">
@@ -1203,8 +1316,32 @@
       <c r="I10" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="L10" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R10" s="9" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1223,8 +1360,32 @@
       <c r="I11" s="9" t="n">
         <v>3</v>
       </c>
+      <c r="L11" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R11" s="9" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="n">
+        <v>13</v>
+      </c>
       <c r="D12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1243,8 +1404,32 @@
       <c r="I12" s="9" t="n">
         <v>5</v>
       </c>
+      <c r="L12" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" s="9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="n">
+        <v>16</v>
+      </c>
       <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1263,8 +1448,32 @@
       <c r="I13" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="L13" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R13" s="9" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="n">
+        <v>18</v>
+      </c>
       <c r="D14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1283,8 +1492,32 @@
       <c r="I14" s="9" t="n">
         <v>1</v>
       </c>
+      <c r="L14" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R14" s="9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="n">
+        <v>19</v>
+      </c>
       <c r="D15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1303,8 +1536,32 @@
       <c r="I15" s="9" t="n">
         <v>4</v>
       </c>
+      <c r="L15" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R15" s="9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="n">
+        <v>21</v>
+      </c>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1323,8 +1580,32 @@
       <c r="I16" s="9" t="n">
         <v>2</v>
       </c>
+      <c r="L16" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R16" s="9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="n">
+        <v>22</v>
+      </c>
       <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
@@ -1343,8 +1624,32 @@
       <c r="I17" s="9" t="n">
         <v>2</v>
       </c>
+      <c r="L17" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R17" s="9" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="n">
+        <v>41</v>
+      </c>
       <c r="D18" s="4" t="s">
         <v>22</v>
       </c>
@@ -1363,8 +1668,32 @@
       <c r="I18" s="9" t="n">
         <v>1</v>
       </c>
+      <c r="L18" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R18" s="9" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="n">
+        <v>320</v>
+      </c>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
@@ -1383,8 +1712,32 @@
       <c r="I19" s="9" t="n">
         <v>4</v>
       </c>
+      <c r="L19" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R19" s="9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="n">
+        <v>150</v>
+      </c>
       <c r="D20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1403,8 +1756,32 @@
       <c r="I20" s="9" t="n">
         <v>3</v>
       </c>
+      <c r="L20" s="0" t="n">
+        <v>276</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R20" s="9" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="n">
+        <v>170</v>
+      </c>
       <c r="D21" s="4" t="s">
         <v>25</v>
       </c>
@@ -1423,8 +1800,32 @@
       <c r="I21" s="9" t="n">
         <v>2</v>
       </c>
+      <c r="L21" s="0" t="n">
+        <v>179</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="n">
+        <v>276</v>
+      </c>
       <c r="D22" s="4" t="s">
         <v>26</v>
       </c>
@@ -1443,8 +1844,32 @@
       <c r="I22" s="9" t="n">
         <v>3</v>
       </c>
+      <c r="L22" s="0" t="n">
+        <v>298</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="n">
+        <v>179</v>
+      </c>
       <c r="D23" s="4" t="s">
         <v>27</v>
       </c>
@@ -1463,8 +1888,32 @@
       <c r="I23" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="L23" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="n">
+        <v>298</v>
+      </c>
       <c r="D24" s="4" t="s">
         <v>28</v>
       </c>
@@ -1485,6 +1934,9 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="0" t="n">
+        <v>184</v>
+      </c>
       <c r="D25" s="4" t="s">
         <v>34</v>
       </c>
@@ -1505,6 +1957,9 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0" t="n">
+        <v>180</v>
+      </c>
       <c r="D26" s="4" t="s">
         <v>35</v>
       </c>
@@ -1525,6 +1980,9 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="n">
+        <v>182</v>
+      </c>
       <c r="D27" s="4" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
novas imagens e resultados
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
@@ -296,8 +296,8 @@
   </sheetPr>
   <dimension ref="D6:T36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N20" activeCellId="1" sqref="M5:R5 N20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R31" activeCellId="0" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,6 +597,12 @@
       <c r="L14" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="M14" s="6" t="n">
+        <v>0.2599</v>
+      </c>
+      <c r="N14" s="6" t="n">
+        <v>0.2454</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="9" t="n">
         <v>921557</v>
@@ -624,6 +630,12 @@
       <c r="L15" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="M15" s="6" t="n">
+        <v>0.3277</v>
+      </c>
+      <c r="N15" s="6" t="n">
+        <v>0.3471</v>
+      </c>
       <c r="Q15" s="1" t="n">
         <v>298611</v>
       </c>
@@ -655,6 +667,12 @@
       </c>
       <c r="L16" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="M16" s="6" t="n">
+        <v>0.2629</v>
+      </c>
+      <c r="N16" s="6" t="n">
+        <v>0.3105</v>
       </c>
       <c r="T16" s="1" t="n">
         <v>175831</v>
@@ -677,6 +695,12 @@
       <c r="L17" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="M17" s="6" t="n">
+        <v>0.2024</v>
+      </c>
+      <c r="N17" s="6" t="n">
+        <v>0.2648</v>
+      </c>
       <c r="T17" s="1" t="n">
         <f aca="false">921600 - SUM(T15:T16)</f>
         <v>11888</v>
@@ -700,6 +724,12 @@
       <c r="L18" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="M18" s="6" t="n">
+        <v>0.1101</v>
+      </c>
+      <c r="N18" s="6" t="n">
+        <v>0.1151</v>
+      </c>
       <c r="T18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,6 +752,12 @@
       </c>
       <c r="L19" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="M19" s="6" t="n">
+        <v>0.2299</v>
+      </c>
+      <c r="N19" s="6" t="n">
+        <v>0.399</v>
       </c>
       <c r="T19" s="1" t="n">
         <v>323160</v>
@@ -744,6 +780,12 @@
       <c r="L20" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="M20" s="6" t="n">
+        <v>0.2193</v>
+      </c>
+      <c r="N20" s="6" t="n">
+        <v>0.2268</v>
+      </c>
       <c r="T20" s="1" t="n">
         <v>527281</v>
       </c>
@@ -766,6 +808,12 @@
       <c r="L21" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="M21" s="6" t="n">
+        <v>0.4112</v>
+      </c>
+      <c r="N21" s="6" t="n">
+        <v>0.4714</v>
+      </c>
       <c r="T21" s="1" t="n">
         <f aca="false">921582 - SUM(T19:T20)</f>
         <v>71141</v>
@@ -791,6 +839,12 @@
       </c>
       <c r="L22" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="M22" s="6" t="n">
+        <v>0.1609</v>
+      </c>
+      <c r="N22" s="6" t="n">
+        <v>0.1815</v>
       </c>
       <c r="T22" s="1"/>
     </row>
@@ -811,6 +865,12 @@
       <c r="L23" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="M23" s="6" t="n">
+        <v>0.3184</v>
+      </c>
+      <c r="N23" s="6" t="n">
+        <v>0.3782</v>
+      </c>
       <c r="T23" s="1" t="n">
         <v>605471</v>
       </c>
@@ -833,6 +893,12 @@
       <c r="L24" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="M24" s="6" t="n">
+        <v>0.3319</v>
+      </c>
+      <c r="N24" s="6" t="n">
+        <v>0.3454</v>
+      </c>
       <c r="T24" s="1" t="n">
         <v>306577</v>
       </c>
@@ -857,6 +923,12 @@
       </c>
       <c r="L25" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="M25" s="6" t="n">
+        <v>0.5561</v>
+      </c>
+      <c r="N25" s="6" t="n">
+        <v>0.6226</v>
       </c>
       <c r="T25" s="1" t="n">
         <f aca="false">921578 - SUM(T23:T24)</f>
@@ -880,6 +952,12 @@
       <c r="L26" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="M26" s="6" t="n">
+        <v>0.2507</v>
+      </c>
+      <c r="N26" s="6" t="n">
+        <v>0.2081</v>
+      </c>
       <c r="T26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,6 +977,12 @@
       </c>
       <c r="L27" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="M27" s="6" t="n">
+        <v>0.3705</v>
+      </c>
+      <c r="N27" s="6" t="n">
+        <v>0.3784</v>
       </c>
       <c r="T27" s="1" t="n">
         <v>321820</v>
@@ -1052,8 +1136,8 @@
   </sheetPr>
   <dimension ref="C4:R29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5:R5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
novos e ultimos resultados
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="90">
   <si>
     <t xml:space="preserve">RGB</t>
   </si>
@@ -42,36 +42,171 @@
     <t xml:space="preserve">Fundo</t>
   </si>
   <si>
+    <t xml:space="preserve">Imagens</t>
+  </si>
+  <si>
     <t xml:space="preserve">AFSoft</t>
   </si>
   <si>
-    <t xml:space="preserve">Visual</t>
+    <t xml:space="preserve">Maioria das estimativas visuais</t>
   </si>
   <si>
     <t xml:space="preserve">Folha</t>
   </si>
   <si>
+    <t xml:space="preserve">Imagem 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,62%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20,43%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-25%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Doença</t>
   </si>
   <si>
+    <t xml:space="preserve">Imagem 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23,09%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26,69%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,67%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inconsistente</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foto 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Imagem 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,13%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42,20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,69%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-12%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,66%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,56%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,47%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,58%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,28%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,06%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foto 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Imagem 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53,23%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64,50%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,29%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-50%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foto 4</t>
   </si>
   <si>
+    <t xml:space="preserve">Imagem 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foto 5</t>
   </si>
   <si>
+    <t xml:space="preserve">Imagem 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 14</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foto 6</t>
   </si>
   <si>
+    <t xml:space="preserve">Imagem 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 17</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foto 7</t>
   </si>
   <si>
+    <t xml:space="preserve">Imagem 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem 20</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foto 8</t>
   </si>
   <si>
@@ -81,6 +216,21 @@
     <t xml:space="preserve">Foto 10</t>
   </si>
   <si>
+    <t xml:space="preserve">Participante 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participante 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participante 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participante 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participante 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foto 11</t>
   </si>
   <si>
@@ -109,21 +259,6 @@
   </si>
   <si>
     <t xml:space="preserve">Foto 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participante 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participante 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participante 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participante 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participante 5</t>
   </si>
   <si>
     <t xml:space="preserve">Foto 21</t>
@@ -163,12 +298,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -195,12 +331,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -246,7 +376,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -263,20 +393,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -284,6 +410,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -306,8 +444,8 @@
   </sheetPr>
   <dimension ref="D6:T36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -319,12 +457,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="7.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="19" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="12" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="15.8"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
   </cols>
@@ -346,7 +480,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
@@ -364,6 +498,9 @@
       <c r="H7" s="0" t="n">
         <v>82.23</v>
       </c>
+      <c r="L7" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="M7" s="4" t="s">
         <v>0</v>
       </c>
@@ -371,19 +508,17 @@
         <v>1</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="T7" s="1" t="n">
-        <v>757273</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="T7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="3"/>
       <c r="E8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>13.28</v>
@@ -395,26 +530,26 @@
         <v>16.67</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" s="5" t="n">
-        <v>0.1762</v>
-      </c>
-      <c r="N8" s="6" t="n">
-        <v>0.2043</v>
-      </c>
-      <c r="O8" s="7" t="n">
-        <v>0.1238</v>
-      </c>
-      <c r="P8" s="6"/>
-      <c r="T8" s="1" t="n">
-        <v>153490</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="3"/>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.84</v>
@@ -427,26 +562,25 @@
         <v>1.09999999999999</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="5" t="n">
-        <v>0.2309</v>
-      </c>
-      <c r="N9" s="5" t="n">
-        <v>0.2669</v>
-      </c>
-      <c r="O9" s="7" t="n">
-        <v>0.0967</v>
-      </c>
-      <c r="P9" s="6"/>
-      <c r="T9" s="1" t="n">
-        <f aca="false">920910 - SUM(T7:T8)</f>
-        <v>10147</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -463,24 +597,26 @@
         <v>57.62</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="5" t="n">
-        <v>0.3213</v>
-      </c>
-      <c r="N10" s="5" t="n">
-        <v>0.422</v>
-      </c>
-      <c r="O10" s="7" t="n">
-        <v>0.0869</v>
-      </c>
-      <c r="P10" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="T10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="3"/>
       <c r="E11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>32.68</v>
@@ -492,33 +628,26 @@
         <v>38.54</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M11" s="5" t="n">
-        <v>0.3166</v>
-      </c>
-      <c r="N11" s="5" t="n">
-        <v>0.3656</v>
-      </c>
-      <c r="O11" s="7" t="n">
-        <v>0.0847</v>
-      </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="0" t="n">
-        <f aca="false">SUM(H26:H27)</f>
-        <v>33.45</v>
-      </c>
-      <c r="R11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="T11" s="1" t="n">
-        <v>530869</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="3"/>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>9.81</v>
@@ -531,32 +660,26 @@
         <v>3.84</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" s="5" t="n">
-        <v>0.3058</v>
-      </c>
-      <c r="N12" s="5" t="n">
-        <v>0.3528</v>
-      </c>
-      <c r="O12" s="7" t="n">
-        <v>0.0206</v>
-      </c>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="0" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="R12" s="8" t="n">
-        <f aca="false">(R11*Q12)/Q11</f>
-        <v>3.1390134529148</v>
-      </c>
-      <c r="T12" s="1" t="n">
-        <v>355075</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" s="7"/>
+      <c r="T12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>5</v>
@@ -573,27 +696,26 @@
         <v>79.63</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="5" t="n">
-        <v>0.5323</v>
-      </c>
-      <c r="N13" s="5" t="n">
-        <v>0.645</v>
-      </c>
-      <c r="O13" s="7" t="n">
-        <v>0.0329</v>
-      </c>
-      <c r="P13" s="6"/>
-      <c r="T13" s="1" t="n">
-        <f aca="false">921359 - SUM(T11:T12)</f>
-        <v>35415</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="3"/>
       <c r="E14" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>13.88</v>
@@ -605,27 +727,21 @@
         <v>19.08</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M14" s="6" t="n">
-        <v>0.2599</v>
-      </c>
-      <c r="N14" s="6" t="n">
-        <v>0.2454</v>
-      </c>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="9" t="n">
-        <v>921557</v>
-      </c>
-      <c r="R14" s="0" t="n">
-        <v>100</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q14" s="8"/>
       <c r="T14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="3"/>
       <c r="E15" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>6.57</v>
@@ -638,28 +754,21 @@
         <v>1.29000000000001</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15" s="6" t="n">
-        <v>0.3277</v>
-      </c>
-      <c r="N15" s="6" t="n">
-        <v>0.3471</v>
-      </c>
-      <c r="Q15" s="1" t="n">
-        <v>298611</v>
-      </c>
-      <c r="R15" s="8" t="n">
-        <f aca="false">(R14*Q15)/Q14</f>
-        <v>32.4028790405802</v>
-      </c>
-      <c r="T15" s="1" t="n">
-        <v>733881</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="7"/>
+      <c r="T15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>5</v>
@@ -676,22 +785,20 @@
         <v>35.07</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M16" s="6" t="n">
-        <v>0.2629</v>
-      </c>
-      <c r="N16" s="6" t="n">
-        <v>0.3105</v>
-      </c>
-      <c r="T16" s="1" t="n">
-        <v>175831</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="3"/>
       <c r="E17" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>44.38</v>
@@ -703,23 +810,20 @@
         <v>57.21</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M17" s="6" t="n">
-        <v>0.2024</v>
-      </c>
-      <c r="N17" s="6" t="n">
-        <v>0.2648</v>
-      </c>
-      <c r="T17" s="1" t="n">
-        <f aca="false">921600 - SUM(T15:T16)</f>
-        <v>11888</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="3"/>
       <c r="E18" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>20.56</v>
@@ -732,19 +836,19 @@
         <v>7.72</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="6" t="n">
-        <v>0.1101</v>
-      </c>
-      <c r="N18" s="6" t="n">
-        <v>0.1151</v>
+        <v>48</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="T18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="3" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>5</v>
@@ -761,22 +865,20 @@
         <v>65.7</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" s="6" t="n">
-        <v>0.2299</v>
-      </c>
-      <c r="N19" s="6" t="n">
-        <v>0.399</v>
-      </c>
-      <c r="T19" s="1" t="n">
-        <v>323160</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="3"/>
       <c r="E20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>23.81</v>
@@ -788,22 +890,20 @@
         <v>33.27</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="6" t="n">
-        <v>0.2193</v>
-      </c>
-      <c r="N20" s="6" t="n">
-        <v>0.2268</v>
-      </c>
-      <c r="T20" s="1" t="n">
-        <v>527281</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="3"/>
       <c r="E21" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>10.49</v>
@@ -816,22 +916,19 @@
         <v>1.03</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" s="6" t="n">
-        <v>0.4112</v>
-      </c>
-      <c r="N21" s="6" t="n">
-        <v>0.4714</v>
-      </c>
-      <c r="T21" s="1" t="n">
-        <f aca="false">921582 - SUM(T19:T20)</f>
-        <v>71141</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="3" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>5</v>
@@ -848,20 +945,20 @@
         <v>34.92</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M22" s="6" t="n">
-        <v>0.1609</v>
-      </c>
-      <c r="N22" s="6" t="n">
-        <v>0.1815</v>
+        <v>54</v>
+      </c>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="T22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="3"/>
       <c r="E23" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>44.52</v>
@@ -873,22 +970,20 @@
         <v>57.03</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" s="6" t="n">
-        <v>0.3184</v>
-      </c>
-      <c r="N23" s="6" t="n">
-        <v>0.3782</v>
-      </c>
-      <c r="T23" s="1" t="n">
-        <v>605471</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="3"/>
       <c r="E24" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>20.56</v>
@@ -901,21 +996,19 @@
         <v>8.05</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M24" s="6" t="n">
-        <v>0.3319</v>
-      </c>
-      <c r="N24" s="6" t="n">
-        <v>0.3454</v>
-      </c>
-      <c r="T24" s="1" t="n">
-        <v>306577</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="3" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>5</v>
@@ -932,23 +1025,20 @@
         <v>66.55</v>
       </c>
       <c r="L25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M25" s="6" t="n">
-        <v>0.5561</v>
-      </c>
-      <c r="N25" s="6" t="n">
-        <v>0.6226</v>
-      </c>
-      <c r="T25" s="1" t="n">
-        <f aca="false">921578 - SUM(T23:T24)</f>
-        <v>9530</v>
-      </c>
+      <c r="T25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="3"/>
       <c r="E26" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>15.64</v>
@@ -960,20 +1050,20 @@
         <v>32.4</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M26" s="6" t="n">
-        <v>0.2507</v>
-      </c>
-      <c r="N26" s="6" t="n">
-        <v>0.2081</v>
+        <v>59</v>
+      </c>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="T26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="3"/>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>17.8</v>
@@ -986,21 +1076,19 @@
         <v>1.05000000000001</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M27" s="6" t="n">
-        <v>0.3705</v>
-      </c>
-      <c r="N27" s="6" t="n">
-        <v>0.3784</v>
-      </c>
-      <c r="T27" s="1" t="n">
-        <v>321820</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="3" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>5</v>
@@ -1013,24 +1101,19 @@
         <f aca="false">100-SUM(G29:G30)</f>
         <v>100</v>
       </c>
-      <c r="T28" s="1" t="n">
-        <v>525551</v>
-      </c>
+      <c r="T28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="3"/>
       <c r="E29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T29" s="1" t="n">
-        <f aca="false">921571 - SUM(T27:T28)</f>
-        <v>74200</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="T29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="3"/>
       <c r="E30" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H30" s="0" t="n">
         <f aca="false">100-SUM(H28:H29)</f>
@@ -1040,7 +1123,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="3" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>5</v>
@@ -1053,36 +1136,29 @@
         <f aca="false">100-SUM(G32:G33)</f>
         <v>100</v>
       </c>
-      <c r="T31" s="1" t="n">
-        <v>613325</v>
-      </c>
+      <c r="T31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="3"/>
       <c r="E32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T32" s="1" t="n">
-        <v>298611</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="T32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="3"/>
       <c r="E33" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H33" s="0" t="n">
         <f aca="false">100-SUM(H31:H32)</f>
         <v>100</v>
       </c>
-      <c r="T33" s="1" t="n">
-        <f aca="false">921557 - SUM(T31:T32)</f>
-        <v>9621</v>
-      </c>
+      <c r="T33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="3" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>5</v>
@@ -1100,14 +1176,14 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D35" s="3"/>
       <c r="E35" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D36" s="3"/>
       <c r="E36" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H36" s="0" t="n">
         <f aca="false">100-SUM(H34:H35)</f>
@@ -1161,22 +1237,22 @@
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="4" t="s">
+      <c r="E4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="N4" s="0" t="n">
@@ -1196,7 +1272,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="0" t="n">
@@ -1217,8 +1293,8 @@
       <c r="L5" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>10</v>
+      <c r="M5" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>5</v>
@@ -1240,8 +1316,8 @@
       <c r="C6" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
+      <c r="D6" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>5</v>
@@ -1258,8 +1334,8 @@
       <c r="I6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>11</v>
+      <c r="M6" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>4</v>
@@ -1278,8 +1354,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="4" t="s">
-        <v>11</v>
+      <c r="D7" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>4</v>
@@ -1296,8 +1372,8 @@
       <c r="I7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>12</v>
+      <c r="M7" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>5</v>
@@ -1316,8 +1392,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="4" t="s">
-        <v>12</v>
+      <c r="D8" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>5</v>
@@ -1334,8 +1410,8 @@
       <c r="I8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>13</v>
+      <c r="M8" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>3</v>
@@ -1354,8 +1430,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="4" t="s">
-        <v>13</v>
+      <c r="D9" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3</v>
@@ -1372,8 +1448,8 @@
       <c r="I9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>14</v>
+      <c r="M9" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>3</v>
@@ -1392,8 +1468,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="4" t="s">
-        <v>14</v>
+      <c r="D10" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>3</v>
@@ -1413,8 +1489,8 @@
       <c r="L10" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="M10" s="4" t="s">
-        <v>15</v>
+      <c r="M10" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>2</v>
@@ -1428,7 +1504,7 @@
       <c r="Q10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="R10" s="9" t="n">
+      <c r="R10" s="8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1436,8 +1512,8 @@
       <c r="C11" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>15</v>
+      <c r="D11" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>2</v>
@@ -1451,14 +1527,14 @@
       <c r="H11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="9" t="n">
+      <c r="I11" s="8" t="n">
         <v>3</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>16</v>
+      <c r="M11" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="N11" s="0" t="n">
         <v>5</v>
@@ -1472,7 +1548,7 @@
       <c r="Q11" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="R11" s="9" t="n">
+      <c r="R11" s="8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1480,8 +1556,8 @@
       <c r="C12" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>16</v>
+      <c r="D12" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>5</v>
@@ -1495,14 +1571,14 @@
       <c r="H12" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I12" s="9" t="n">
+      <c r="I12" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="M12" s="4" t="s">
-        <v>17</v>
+      <c r="M12" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>1</v>
@@ -1516,7 +1592,7 @@
       <c r="Q12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="R12" s="9" t="n">
+      <c r="R12" s="8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1524,8 +1600,8 @@
       <c r="C13" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>17</v>
+      <c r="D13" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>4</v>
@@ -1545,8 +1621,8 @@
       <c r="L13" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>18</v>
+      <c r="M13" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="N13" s="0" t="n">
         <v>4</v>
@@ -1560,7 +1636,7 @@
       <c r="Q13" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="R13" s="9" t="n">
+      <c r="R13" s="8" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1568,8 +1644,8 @@
       <c r="C14" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>18</v>
+      <c r="D14" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
@@ -1583,14 +1659,14 @@
       <c r="H14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="9" t="n">
+      <c r="I14" s="8" t="n">
         <v>1</v>
       </c>
       <c r="L14" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="M14" s="4" t="s">
-        <v>19</v>
+      <c r="M14" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="N14" s="0" t="n">
         <v>3</v>
@@ -1604,7 +1680,7 @@
       <c r="Q14" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="R14" s="9" t="n">
+      <c r="R14" s="8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1612,8 +1688,8 @@
       <c r="C15" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>19</v>
+      <c r="D15" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>4</v>
@@ -1627,14 +1703,14 @@
       <c r="H15" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I15" s="9" t="n">
+      <c r="I15" s="8" t="n">
         <v>4</v>
       </c>
       <c r="L15" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="M15" s="4" t="s">
-        <v>20</v>
+      <c r="M15" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="N15" s="0" t="n">
         <v>1</v>
@@ -1648,7 +1724,7 @@
       <c r="Q15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="R15" s="9" t="n">
+      <c r="R15" s="8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1656,8 +1732,8 @@
       <c r="C16" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>20</v>
+      <c r="D16" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>3</v>
@@ -1671,14 +1747,14 @@
       <c r="H16" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I16" s="9" t="n">
+      <c r="I16" s="8" t="n">
         <v>2</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="M16" s="4" t="s">
-        <v>21</v>
+      <c r="M16" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="N16" s="0" t="n">
         <v>2</v>
@@ -1692,7 +1768,7 @@
       <c r="Q16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="R16" s="9" t="n">
+      <c r="R16" s="8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1700,8 +1776,8 @@
       <c r="C17" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>21</v>
+      <c r="D17" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
@@ -1715,14 +1791,14 @@
       <c r="H17" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I17" s="9" t="n">
+      <c r="I17" s="8" t="n">
         <v>2</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>320</v>
       </c>
-      <c r="M17" s="4" t="s">
-        <v>22</v>
+      <c r="M17" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="N17" s="0" t="n">
         <v>3</v>
@@ -1736,7 +1812,7 @@
       <c r="Q17" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="R17" s="9" t="n">
+      <c r="R17" s="8" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1744,8 +1820,8 @@
       <c r="C18" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>22</v>
+      <c r="D18" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>2</v>
@@ -1759,14 +1835,14 @@
       <c r="H18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I18" s="9" t="n">
+      <c r="I18" s="8" t="n">
         <v>1</v>
       </c>
       <c r="L18" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="M18" s="4" t="s">
-        <v>23</v>
+      <c r="M18" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>3</v>
@@ -1780,7 +1856,7 @@
       <c r="Q18" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="R18" s="9" t="n">
+      <c r="R18" s="8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1788,8 +1864,8 @@
       <c r="C19" s="0" t="n">
         <v>320</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>23</v>
+      <c r="D19" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>3</v>
@@ -1803,14 +1879,14 @@
       <c r="H19" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I19" s="9" t="n">
+      <c r="I19" s="8" t="n">
         <v>4</v>
       </c>
       <c r="L19" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="M19" s="4" t="s">
-        <v>24</v>
+      <c r="M19" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>2</v>
@@ -1824,7 +1900,7 @@
       <c r="Q19" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="R19" s="9" t="n">
+      <c r="R19" s="8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1832,8 +1908,8 @@
       <c r="C20" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>24</v>
+      <c r="D20" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>3</v>
@@ -1847,14 +1923,14 @@
       <c r="H20" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I20" s="9" t="n">
+      <c r="I20" s="8" t="n">
         <v>3</v>
       </c>
       <c r="L20" s="0" t="n">
         <v>276</v>
       </c>
-      <c r="M20" s="4" t="s">
-        <v>25</v>
+      <c r="M20" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>3</v>
@@ -1868,7 +1944,7 @@
       <c r="Q20" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="R20" s="9" t="n">
+      <c r="R20" s="8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1876,8 +1952,8 @@
       <c r="C21" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>25</v>
+      <c r="D21" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>2</v>
@@ -1891,14 +1967,14 @@
       <c r="H21" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I21" s="9" t="n">
+      <c r="I21" s="8" t="n">
         <v>2</v>
       </c>
       <c r="L21" s="0" t="n">
         <v>179</v>
       </c>
-      <c r="M21" s="4" t="s">
-        <v>26</v>
+      <c r="M21" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="N21" s="0" t="n">
         <v>2</v>
@@ -1920,8 +1996,8 @@
       <c r="C22" s="0" t="n">
         <v>276</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>26</v>
+      <c r="D22" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>3</v>
@@ -1935,14 +2011,14 @@
       <c r="H22" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I22" s="9" t="n">
+      <c r="I22" s="8" t="n">
         <v>3</v>
       </c>
       <c r="L22" s="0" t="n">
         <v>298</v>
       </c>
-      <c r="M22" s="4" t="s">
-        <v>27</v>
+      <c r="M22" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>5</v>
@@ -1964,8 +2040,8 @@
       <c r="C23" s="0" t="n">
         <v>179</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>27</v>
+      <c r="D23" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>2</v>
@@ -1985,8 +2061,8 @@
       <c r="L23" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="M23" s="4" t="s">
-        <v>28</v>
+      <c r="M23" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="N23" s="0" t="n">
         <v>3</v>
@@ -2008,8 +2084,8 @@
       <c r="C24" s="0" t="n">
         <v>298</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>28</v>
+      <c r="D24" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>5</v>
@@ -2031,8 +2107,8 @@
       <c r="C25" s="0" t="n">
         <v>184</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>34</v>
+      <c r="D25" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>5</v>
@@ -2054,8 +2130,8 @@
       <c r="C26" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>35</v>
+      <c r="D26" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>3</v>
@@ -2077,8 +2153,8 @@
       <c r="C27" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>36</v>
+      <c r="D27" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>3</v>
@@ -2098,19 +2174,19 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="0" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2129,10 +2205,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D6:M27"/>
+  <dimension ref="D6:P27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2142,566 +2218,586 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="7.73"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="7.73"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="11" style="0" width="7.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="K6" s="2" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="N6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>0.1762</v>
+      </c>
+      <c r="F8" s="10" t="n">
+        <v>0.0608</v>
+      </c>
+      <c r="G8" s="10" t="n">
+        <v>0.0505</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="M8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="11" t="n">
+        <v>0.2043</v>
+      </c>
+      <c r="O8" s="11" t="n">
+        <v>0.1504</v>
+      </c>
+      <c r="P8" s="11" t="n">
+        <v>0.0646</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>0.2309</v>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>0.1062</v>
+      </c>
+      <c r="G9" s="10" t="n">
+        <v>0.0683</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="M9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="11" t="n">
+        <v>0.2669</v>
+      </c>
+      <c r="O9" s="11" t="n">
+        <v>0.1236</v>
+      </c>
+      <c r="P9" s="11" t="n">
+        <v>0.084</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>0.3213</v>
+      </c>
+      <c r="F10" s="10" t="n">
+        <v>0.1178</v>
+      </c>
+      <c r="G10" s="10" t="n">
+        <v>0.0714</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="M10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="11" t="n">
+        <v>0.422</v>
+      </c>
+      <c r="O10" s="11" t="n">
+        <v>0.1241</v>
+      </c>
+      <c r="P10" s="11" t="n">
+        <v>0.0797</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="4" t="s">
+      <c r="E11" s="10" t="n">
+        <v>0.3166</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <v>0.1708</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>0.0801</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="M11" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>0.1762</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>0.0608</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>0.0505</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="6" t="n">
-        <v>0.2043</v>
-      </c>
-      <c r="L8" s="6" t="n">
-        <v>0.1504</v>
-      </c>
-      <c r="M8" s="6" t="n">
-        <v>0.0646</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>0.2309</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0.1062</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <v>0.0683</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="6" t="n">
-        <v>0.2669</v>
-      </c>
-      <c r="L9" s="6" t="n">
-        <v>0.1236</v>
-      </c>
-      <c r="M9" s="6" t="n">
-        <v>0.084</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>0.3213</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>0.1178</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>0.0714</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="6" t="n">
-        <v>0.422</v>
-      </c>
-      <c r="L10" s="6" t="n">
-        <v>0.1241</v>
-      </c>
-      <c r="M10" s="6" t="n">
-        <v>0.0797</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <v>0.3166</v>
-      </c>
-      <c r="F11" s="5" t="n">
-        <v>0.1708</v>
-      </c>
-      <c r="G11" s="5" t="n">
-        <v>0.0801</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="6" t="n">
+      <c r="N11" s="11" t="n">
         <v>0.3656</v>
       </c>
-      <c r="L11" s="6" t="n">
+      <c r="O11" s="11" t="n">
         <v>0.2033</v>
       </c>
-      <c r="M11" s="6" t="n">
+      <c r="P11" s="11" t="n">
         <v>0.0973</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="5" t="n">
+      <c r="D12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="10" t="n">
         <v>0.3058</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="F12" s="10" t="n">
         <v>0.1</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="10" t="n">
         <v>0.0528</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="6" t="n">
+      <c r="H12" s="6"/>
+      <c r="M12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="11" t="n">
         <v>0.3528</v>
       </c>
-      <c r="L12" s="6" t="n">
+      <c r="O12" s="11" t="n">
         <v>0.1105</v>
       </c>
-      <c r="M12" s="6" t="n">
+      <c r="P12" s="11" t="n">
         <v>0.0449</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="5" t="n">
+      <c r="D13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="10" t="n">
         <v>0.5323</v>
       </c>
-      <c r="F13" s="5" t="n">
+      <c r="F13" s="10" t="n">
         <v>0.0586</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="G13" s="10" t="n">
         <v>0.0395</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="6" t="n">
+      <c r="H13" s="6"/>
+      <c r="M13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N13" s="11" t="n">
         <v>0.645</v>
       </c>
-      <c r="L13" s="6" t="n">
+      <c r="O13" s="11" t="n">
         <v>0.0984</v>
       </c>
-      <c r="M13" s="6" t="n">
+      <c r="P13" s="11" t="n">
         <v>0.0481</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="5" t="n">
+      <c r="D14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="10" t="n">
         <v>0.2599</v>
       </c>
-      <c r="F14" s="5" t="n">
+      <c r="F14" s="10" t="n">
         <v>0.0977</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="G14" s="10" t="n">
         <v>0.048</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="6" t="n">
+      <c r="H14" s="6"/>
+      <c r="M14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N14" s="11" t="n">
         <v>0.2454</v>
       </c>
-      <c r="L14" s="6" t="n">
+      <c r="O14" s="11" t="n">
         <v>0.099</v>
       </c>
-      <c r="M14" s="6" t="n">
+      <c r="P14" s="11" t="n">
         <v>0.0476</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="5" t="n">
+      <c r="D15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="10" t="n">
         <v>0.3277</v>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="10" t="n">
         <v>0.1495</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="10" t="n">
         <v>0.102</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="6" t="n">
+      <c r="H15" s="6"/>
+      <c r="M15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N15" s="11" t="n">
         <v>0.3471</v>
       </c>
-      <c r="L15" s="6" t="n">
+      <c r="O15" s="11" t="n">
         <v>0.1836</v>
       </c>
-      <c r="M15" s="6" t="n">
+      <c r="P15" s="11" t="n">
         <v>0.1297</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="5" t="n">
+      <c r="D16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="10" t="n">
         <v>0.2629</v>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="F16" s="10" t="n">
         <v>0.1101</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="10" t="n">
         <v>0.0664</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="6" t="n">
+      <c r="H16" s="6"/>
+      <c r="M16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" s="11" t="n">
         <v>0.3105</v>
       </c>
-      <c r="L16" s="6" t="n">
+      <c r="O16" s="11" t="n">
         <v>0.1165</v>
       </c>
-      <c r="M16" s="6" t="n">
+      <c r="P16" s="11" t="n">
         <v>0.0702</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="5" t="n">
+      <c r="D17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="10" t="n">
         <v>0.2024</v>
       </c>
-      <c r="F17" s="5" t="n">
+      <c r="F17" s="10" t="n">
         <v>0.0449</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" s="10" t="n">
         <v>0.0307</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="6" t="n">
+      <c r="H17" s="6"/>
+      <c r="M17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N17" s="11" t="n">
         <v>0.2648</v>
       </c>
-      <c r="L17" s="6" t="n">
+      <c r="O17" s="11" t="n">
         <v>0.1119</v>
       </c>
-      <c r="M17" s="6" t="n">
+      <c r="P17" s="11" t="n">
         <v>0.0386</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="5" t="n">
+      <c r="D18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="10" t="n">
         <v>0.1101</v>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="F18" s="10" t="n">
         <v>0.0159</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" s="10" t="n">
         <v>0.0149</v>
       </c>
-      <c r="J18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K18" s="6" t="n">
+      <c r="H18" s="6"/>
+      <c r="M18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="N18" s="11" t="n">
         <v>0.1151</v>
       </c>
-      <c r="L18" s="6" t="n">
+      <c r="O18" s="11" t="n">
         <v>0.0635</v>
       </c>
-      <c r="M18" s="6" t="n">
+      <c r="P18" s="11" t="n">
         <v>0.0228</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="5" t="n">
+      <c r="D19" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="10" t="n">
         <v>0.2299</v>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="F19" s="10" t="n">
         <v>0.0959</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" s="10" t="n">
         <v>0.0347</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="6" t="n">
+      <c r="H19" s="6"/>
+      <c r="M19" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N19" s="11" t="n">
         <v>0.399</v>
       </c>
-      <c r="L19" s="6" t="n">
+      <c r="O19" s="11" t="n">
         <v>0.0955</v>
       </c>
-      <c r="M19" s="6" t="n">
+      <c r="P19" s="11" t="n">
         <v>0.064</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="5" t="n">
+      <c r="D20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="10" t="n">
         <v>0.2193</v>
       </c>
-      <c r="F20" s="5" t="n">
+      <c r="F20" s="10" t="n">
         <v>0.1001</v>
       </c>
-      <c r="G20" s="5" t="n">
+      <c r="G20" s="10" t="n">
         <v>0.0367</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="6" t="n">
+      <c r="H20" s="6"/>
+      <c r="M20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N20" s="11" t="n">
         <v>0.2268</v>
       </c>
-      <c r="L20" s="6" t="n">
+      <c r="O20" s="11" t="n">
         <v>0.1041</v>
       </c>
-      <c r="M20" s="6" t="n">
+      <c r="P20" s="11" t="n">
         <v>0.0493</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="5" t="n">
+      <c r="D21" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="10" t="n">
         <v>0.4112</v>
       </c>
-      <c r="F21" s="5" t="n">
+      <c r="F21" s="10" t="n">
         <v>0.1153</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" s="10" t="n">
         <v>0.0534</v>
       </c>
-      <c r="J21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" s="6" t="n">
+      <c r="H21" s="6"/>
+      <c r="M21" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="N21" s="11" t="n">
         <v>0.4714</v>
       </c>
-      <c r="L21" s="6" t="n">
+      <c r="O21" s="11" t="n">
         <v>0.0951</v>
       </c>
-      <c r="M21" s="6" t="n">
+      <c r="P21" s="11" t="n">
         <v>0.0518</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="5" t="n">
+      <c r="D22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="10" t="n">
         <v>0.1609</v>
       </c>
-      <c r="F22" s="5" t="n">
+      <c r="F22" s="10" t="n">
         <v>0.0458</v>
       </c>
-      <c r="G22" s="5" t="n">
+      <c r="G22" s="10" t="n">
         <v>0.0415</v>
       </c>
-      <c r="J22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="6" t="n">
+      <c r="H22" s="6"/>
+      <c r="M22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="N22" s="11" t="n">
         <v>0.1815</v>
       </c>
-      <c r="L22" s="6" t="n">
+      <c r="O22" s="11" t="n">
         <v>0.0952</v>
       </c>
-      <c r="M22" s="6" t="n">
+      <c r="P22" s="11" t="n">
         <v>0.057</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="5" t="n">
+      <c r="D23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="10" t="n">
         <v>0.3184</v>
       </c>
-      <c r="F23" s="5" t="n">
+      <c r="F23" s="10" t="n">
         <v>0.0899</v>
       </c>
-      <c r="G23" s="5" t="n">
+      <c r="G23" s="10" t="n">
         <v>0.0462</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" s="6" t="n">
+      <c r="H23" s="6"/>
+      <c r="M23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N23" s="11" t="n">
         <v>0.3782</v>
       </c>
-      <c r="L23" s="6" t="n">
+      <c r="O23" s="11" t="n">
         <v>0.099</v>
       </c>
-      <c r="M23" s="6" t="n">
+      <c r="P23" s="11" t="n">
         <v>0.0503</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="5" t="n">
+      <c r="D24" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="10" t="n">
         <v>0.3319</v>
       </c>
-      <c r="F24" s="5" t="n">
+      <c r="F24" s="10" t="n">
         <v>0.0097</v>
       </c>
-      <c r="G24" s="5" t="n">
+      <c r="G24" s="10" t="n">
         <v>0.0086</v>
       </c>
-      <c r="J24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="6" t="n">
+      <c r="H24" s="6"/>
+      <c r="M24" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N24" s="11" t="n">
         <v>0.3454</v>
       </c>
-      <c r="L24" s="6" t="n">
+      <c r="O24" s="11" t="n">
         <v>0.0758</v>
       </c>
-      <c r="M24" s="6" t="n">
+      <c r="P24" s="11" t="n">
         <v>0.0093</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="5" t="n">
+      <c r="D25" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="10" t="n">
         <v>0.5561</v>
       </c>
-      <c r="F25" s="5" t="n">
+      <c r="F25" s="10" t="n">
         <v>0.0886</v>
       </c>
-      <c r="G25" s="5" t="n">
+      <c r="G25" s="10" t="n">
         <v>0.0592</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K25" s="6" t="n">
+      <c r="H25" s="6"/>
+      <c r="M25" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N25" s="11" t="n">
         <v>0.6226</v>
       </c>
-      <c r="L25" s="6" t="n">
+      <c r="O25" s="11" t="n">
         <v>0.187</v>
       </c>
-      <c r="M25" s="6" t="n">
+      <c r="P25" s="11" t="n">
         <v>0.0718</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="5" t="n">
+      <c r="D26" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="10" t="n">
         <v>0.2507</v>
       </c>
-      <c r="F26" s="5" t="n">
+      <c r="F26" s="10" t="n">
         <v>0.0377</v>
       </c>
-      <c r="G26" s="5" t="n">
+      <c r="G26" s="10" t="n">
         <v>0.0372</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K26" s="6" t="n">
+      <c r="H26" s="6"/>
+      <c r="M26" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N26" s="11" t="n">
         <v>0.2081</v>
       </c>
-      <c r="L26" s="6" t="n">
+      <c r="O26" s="11" t="n">
         <v>0.0529</v>
       </c>
-      <c r="M26" s="6" t="n">
+      <c r="P26" s="11" t="n">
         <v>0.0367</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="5" t="n">
+      <c r="D27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="10" t="n">
         <v>0.3705</v>
       </c>
-      <c r="F27" s="5" t="n">
+      <c r="F27" s="10" t="n">
         <v>0.0707</v>
       </c>
-      <c r="G27" s="5" t="n">
+      <c r="G27" s="10" t="n">
         <v>0.0528</v>
       </c>
-      <c r="J27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K27" s="6" t="n">
+      <c r="H27" s="6"/>
+      <c r="M27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="N27" s="11" t="n">
         <v>0.3784</v>
       </c>
-      <c r="L27" s="6" t="n">
+      <c r="O27" s="11" t="n">
         <v>0.089</v>
       </c>
-      <c r="M27" s="6" t="n">
+      <c r="P27" s="11" t="n">
         <v>0.0572</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E6:G6"/>
-    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>